<commit_message>
Reference File Excel sheet
</commit_message>
<xml_diff>
--- a/Referencefile.xlsx
+++ b/Referencefile.xlsx
@@ -861,11 +861,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy\ hh:mm"/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -877,7 +877,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -891,42 +891,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -942,32 +914,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,6 +937,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -997,7 +954,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1006,7 +963,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1015,6 +979,42 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1029,7 +1029,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1041,7 +1065,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1053,13 +1077,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,37 +1107,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1149,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,31 +1197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,49 +1209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,27 +1239,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1297,6 +1286,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1306,17 +1310,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1325,148 +1325,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1475,7 +1475,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1798,7 +1798,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>